<commit_message>
IKD update: GaN CMOS 2026-02-01T23:29Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T118"/>
+  <dimension ref="A1:T119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9319,6 +9319,82 @@
       </c>
       <c r="T118" t="inlineStr"/>
     </row>
+    <row r="119">
+      <c r="A119" t="inlineStr"/>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Fabrication of hierarchical porous chitosan/polyphosphazene monolithic aerogels for efficient iodine adsorption</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Desalination</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Tang, Xiaohuan; Zhang, Jinying; Chu, Huiyuan; Shen, Jiwei; Wang, Chaozhan; Wei, Yinmao</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>10.1016/j.desal.2026.119924</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.desal.2026.119924</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr"/>
+      <c r="O119" t="inlineStr"/>
+      <c r="P119" t="inlineStr"/>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>Fabrication of hierarchical porous chitosan/polyphosphazene monolithic aerogels for efficient iodine adsorption</t>
+        </is>
+      </c>
+      <c r="R119" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="T119" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-02T23:32Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T119"/>
+  <dimension ref="A1:T120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9395,6 +9395,78 @@
       </c>
       <c r="T119" t="inlineStr"/>
     </row>
+    <row r="120">
+      <c r="A120" t="inlineStr"/>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>32.768 kHz Real-Time Oscillator in a General-Purpose Microcontroller Environment Whatever the Quartz Crystal</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Brun, Marine; Jacquemod, Gilles; Charlon, Yoann; Fevre, Philippe Le</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>10.21203/rs.3.rs-7650263/v1</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.21203/rs.3.rs-7650263/v1</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" t="inlineStr"/>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>32.768 kHz Real-Time Oscillator in a General-Purpose Microcontroller Environment Whatever the Quartz Crystal</t>
+        </is>
+      </c>
+      <c r="R120" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>2026-02-02</t>
+        </is>
+      </c>
+      <c r="T120" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-03T23:31Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T120"/>
+  <dimension ref="A1:T127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9467,6 +9467,538 @@
       </c>
       <c r="T120" t="inlineStr"/>
     </row>
+    <row r="121">
+      <c r="A121" t="inlineStr"/>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Low Power Design of CMOS Operational Amplifiers for IoT Edge Devices</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>EWA Publishing</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Applied and Computational Engineering</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Zhou, Huayi</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>10.54254/2755-2721/2026.bj31634</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.54254/2755-2721/2026.bj31634</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" t="inlineStr"/>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>Low Power Design of CMOS Operational Amplifiers for IoT Edge Devices</t>
+        </is>
+      </c>
+      <c r="R121" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="T121" t="inlineStr"/>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr"/>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>MELEGROS: Monolithic Elephant‐Inspired Gripper with Optical Sensors</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Wiley</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Advanced Science</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Trunin, Petr; Cafiso, Diana; Nardin, Anderson Brazil; Exley, Trevor; Beccai, Lucia</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>10.1002/advs.202518878</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/advs.202518878</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" t="inlineStr"/>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>MELEGROS: Monolithic Elephant‐Inspired Gripper with Optical Sensors</t>
+        </is>
+      </c>
+      <c r="R122" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="T122" t="inlineStr"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr"/>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Pin-Plane Electrical Discharge Driven by a MOSFET DC Current Source</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Plasma</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Perry, Myles; Holoman, Sidmar; Wozniak, Daniel; Dhali, Shirshak Kumar</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>10.3390/plasma9010005</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/plasma9010005</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" t="inlineStr"/>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>Pin-Plane Electrical Discharge Driven by a MOSFET DC Current Source</t>
+        </is>
+      </c>
+      <c r="R123" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="T123" t="inlineStr"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr"/>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Pin-Plane Electrical Discharge Driven by a MOSFET DC Current Source</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Plasma</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Perry, Myles; Holoman, Sidmar; Wozniak, Daniel; Dhali, Shirshak Kumar</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>10.3390/plasma9010005</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/plasma9010005</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" t="inlineStr"/>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>Pin-Plane Electrical Discharge Driven by a MOSFET DC Current Source</t>
+        </is>
+      </c>
+      <c r="R124" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="T124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr"/>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Future VLSI Architectures for Neuromorphic Computing, Edge AI and Sustainable Systems</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>2027</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Chandigarh Philosophers</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>International Journal for Multidimensional Research Perspectives</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>R Bhaskar Nihal Varma</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>10.61877/ijmrp.v3i7.293</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.61877/ijmrp.v3i7.293</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N125" t="inlineStr"/>
+      <c r="O125" t="inlineStr"/>
+      <c r="P125" t="inlineStr"/>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>Future VLSI Architectures for Neuromorphic Computing, Edge AI and Sustainable Systems</t>
+        </is>
+      </c>
+      <c r="R125" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="T125" t="inlineStr"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr"/>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Low Power Design of CMOS Operational Amplifiers for IoT Edge Devices</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>EWA Publishing</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Applied and Computational Engineering</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Zhou, Huayi</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>10.54254/2755-2721/2026.bj31634</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.54254/2755-2721/2026.bj31634</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N126" t="inlineStr"/>
+      <c r="O126" t="inlineStr"/>
+      <c r="P126" t="inlineStr"/>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>Low Power Design of CMOS Operational Amplifiers for IoT Edge Devices</t>
+        </is>
+      </c>
+      <c r="R126" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="T126" t="inlineStr"/>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr"/>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Interface dipole modulation for gate dielectrics in Field-Effect transistors: a review</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Journal of the Korean Ceramic Society</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Lim, Wangseop; Kim, Hyojung; Jang, Ho Won</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>10.1007/s43207-026-00587-5</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s43207-026-00587-5</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N127" t="inlineStr"/>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" t="inlineStr"/>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>Interface dipole modulation for gate dielectrics in Field-Effect transistors: a review</t>
+        </is>
+      </c>
+      <c r="R127" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>2026-02-03</t>
+        </is>
+      </c>
+      <c r="T127" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-04T23:32Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T127"/>
+  <dimension ref="A1:T135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9999,6 +9999,614 @@
       </c>
       <c r="T127" t="inlineStr"/>
     </row>
+    <row r="128">
+      <c r="A128" t="inlineStr"/>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Synthesis of Sliding Mode Control Strategy for T-Type Grid Inverter in Presence Grid Voltage Disturbance</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Sawiński, Albert; Chudzik, Piotr; Tatar, Karol</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>10.3390/en19030790</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19030790</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N128" t="inlineStr"/>
+      <c r="O128" t="inlineStr"/>
+      <c r="P128" t="inlineStr"/>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>Synthesis of Sliding Mode Control Strategy for T-Type Grid Inverter in Presence Grid Voltage Disturbance</t>
+        </is>
+      </c>
+      <c r="R128" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S128" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr"/>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>A comparative review of impact-induced failure mechanisms in monolithic and hybrid structures</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Results in Engineering</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Zhong, Zhenhang; Wang, Jiacong</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>10.1016/j.rineng.2026.109340</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.rineng.2026.109340</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>Hybrid</t>
+        </is>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>Integration</t>
+        </is>
+      </c>
+      <c r="N129" t="inlineStr"/>
+      <c r="O129" t="inlineStr"/>
+      <c r="P129" t="inlineStr"/>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>A comparative review of impact-induced failure mechanisms in monolithic and hybrid structures</t>
+        </is>
+      </c>
+      <c r="R129" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S129" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr"/>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Highly Sensitive Room-Temperature Graphene-Modulated AlGaN/GaN HEMT THz Detector Architecture</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Sensors</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Sengupta, Rudrarup; Sarusi, Gabby</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>10.3390/s26031006</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/s26031006</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>Highly Sensitive Room-Temperature Graphene-Modulated AlGaN/GaN HEMT THz Detector Architecture</t>
+        </is>
+      </c>
+      <c r="R130" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S130" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T130" t="inlineStr"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr"/>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Highly Sensitive Room-Temperature Graphene-Modulated AlGaN/GaN HEMT THz Detector Architecture</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Sensors</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Sengupta, Rudrarup; Sarusi, Gabby</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>10.3390/s26031006</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/s26031006</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>Highly Sensitive Room-Temperature Graphene-Modulated AlGaN/GaN HEMT THz Detector Architecture</t>
+        </is>
+      </c>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T131" t="inlineStr"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr"/>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Highly Sensitive Room-Temperature Graphene-Modulated AlGaN/GaN HEMT THz Detector Architecture</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Sensors</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Sengupta, Rudrarup; Sarusi, Gabby</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>10.3390/s26031006</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/s26031006</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N132" t="inlineStr"/>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" t="inlineStr"/>
+      <c r="Q132" t="inlineStr">
+        <is>
+          <t>Highly Sensitive Room-Temperature Graphene-Modulated AlGaN/GaN HEMT THz Detector Architecture</t>
+        </is>
+      </c>
+      <c r="R132" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T132" t="inlineStr"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr"/>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Synthesis of Sliding Mode Control Strategy for T-Type Grid Inverter in Presence Grid Voltage Disturbance</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Sawiński, Albert; Chudzik, Piotr; Tatar, Karol</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>10.3390/en19030790</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19030790</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N133" t="inlineStr"/>
+      <c r="O133" t="inlineStr"/>
+      <c r="P133" t="inlineStr"/>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>Synthesis of Sliding Mode Control Strategy for T-Type Grid Inverter in Presence Grid Voltage Disturbance</t>
+        </is>
+      </c>
+      <c r="R133" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S133" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr"/>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Assessment of an FPGA Implementation of a Hybrid PUF Based on a Configurable Transient Effect Ring Oscillator and Ring Oscillator (TERORO-PUF)</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Casado-Galán, Alejandro; Núñez, Juan; Tena-Sánchez, Erica; Potestad-Ordóñez, Francisco Eugenio; Acosta, Antonio José</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15030661</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15030661</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N134" t="inlineStr"/>
+      <c r="O134" t="inlineStr"/>
+      <c r="P134" t="inlineStr"/>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>Assessment of an FPGA Implementation of a Hybrid PUF Based on a Configurable Transient Effect Ring Oscillator and Ring Oscillator (TERORO-PUF)</t>
+        </is>
+      </c>
+      <c r="R134" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T134" t="inlineStr"/>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr"/>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Synthesis of Sliding Mode Control Strategy for T-Type Grid Inverter in Presence Grid Voltage Disturbance</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Sawiński, Albert; Chudzik, Piotr; Tatar, Karol</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>10.3390/en19030790</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19030790</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N135" t="inlineStr"/>
+      <c r="O135" t="inlineStr"/>
+      <c r="P135" t="inlineStr"/>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>Synthesis of Sliding Mode Control Strategy for T-Type Grid Inverter in Presence Grid Voltage Disturbance</t>
+        </is>
+      </c>
+      <c r="R135" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="T135" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-05T23:27Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T135"/>
+  <dimension ref="A1:T140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10607,6 +10607,386 @@
       </c>
       <c r="T135" t="inlineStr"/>
     </row>
+    <row r="136">
+      <c r="A136" t="inlineStr"/>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Advancements in MOSFET Channel Materials a Comparative Review</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Trans Tech Publications, Ltd.</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Advanced Materials Research</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Sania, Sania; Gangwani, Parvesh; Mohil, Meenu; Kaur, Ravneet</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>10.4028/p-pou2qy</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4028/p-pou2qy</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr"/>
+      <c r="P136" t="inlineStr"/>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>Advancements in MOSFET Channel Materials a Comparative Review</t>
+        </is>
+      </c>
+      <c r="R136" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="T136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr"/>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>FinFET vs Planar MOSFET: A Performance-Based Comparative Study</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Trans Tech Publications, Ltd.</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Advanced Materials Research</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Sahu, Soumya; Saikia, Tanmoi; Gangwani, Parvesh; Kaur, Ravneet</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr"/>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>10.4028/p-1pyqh5</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4028/p-1pyqh5</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N137" t="inlineStr"/>
+      <c r="O137" t="inlineStr"/>
+      <c r="P137" t="inlineStr"/>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>FinFET vs Planar MOSFET: A Performance-Based Comparative Study</t>
+        </is>
+      </c>
+      <c r="R137" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="T137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr"/>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Advancements in MOSFET Channel Materials a Comparative Review</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Trans Tech Publications, Ltd.</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Advanced Materials Research</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Sania, Sania; Gangwani, Parvesh; Mohil, Meenu; Kaur, Ravneet</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>10.4028/p-pou2qy</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4028/p-pou2qy</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N138" t="inlineStr"/>
+      <c r="O138" t="inlineStr"/>
+      <c r="P138" t="inlineStr"/>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>Advancements in MOSFET Channel Materials a Comparative Review</t>
+        </is>
+      </c>
+      <c r="R138" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="T138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr"/>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>FinFET vs Planar MOSFET: A Performance-Based Comparative Study</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Trans Tech Publications, Ltd.</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Advanced Materials Research</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Sahu, Soumya; Saikia, Tanmoi; Gangwani, Parvesh; Kaur, Ravneet</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>10.4028/p-1pyqh5</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.4028/p-1pyqh5</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N139" t="inlineStr"/>
+      <c r="O139" t="inlineStr"/>
+      <c r="P139" t="inlineStr"/>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>FinFET vs Planar MOSFET: A Performance-Based Comparative Study</t>
+        </is>
+      </c>
+      <c r="R139" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="T139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr"/>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Advances in Semiconductor Optical Amplifier Technologies for All-Optical Logic Gate Implementations: A Comprehensive Review</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Nanomaterials</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Cui, Jiali; Zoiros, Kyriakos E.; Kotb, Amer</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>10.3390/nano16030202</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/nano16030202</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N140" t="inlineStr"/>
+      <c r="O140" t="inlineStr"/>
+      <c r="P140" t="inlineStr"/>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>Advances in Semiconductor Optical Amplifier Technologies for All-Optical Logic Gate Implementations: A Comprehensive Review</t>
+        </is>
+      </c>
+      <c r="R140" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="T140" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-06T23:29Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T140"/>
+  <dimension ref="A1:T154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10987,6 +10987,1058 @@
       </c>
       <c r="T140" t="inlineStr"/>
     </row>
+    <row r="141">
+      <c r="A141" t="inlineStr"/>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Wiley</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>physica status solidi (a)</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Then, Han Wui; Zubair, Ahmad; Bader, Samuel; Koirala, Pratik; Beumer, Michael; Vora, Heli; Golani, Prafful; Radosavljevic, Marko</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N141" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
+      <c r="P141" t="inlineStr"/>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="R141" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr"/>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr"/>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>ENI, FAVOUR</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N142" t="inlineStr"/>
+      <c r="O142" t="inlineStr"/>
+      <c r="P142" t="inlineStr"/>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="R142" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr"/>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Wang, Rutian; Wei, Jiahui; Yu, Yang</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N143" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
+      <c r="P143" t="inlineStr"/>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="R143" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T143" t="inlineStr"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr"/>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>ENI, FAVOUR</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N144" t="inlineStr"/>
+      <c r="O144" t="inlineStr"/>
+      <c r="P144" t="inlineStr"/>
+      <c r="Q144" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="R144" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T144" t="inlineStr"/>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr"/>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Wang, Rutian; Wei, Jiahui; Yu, Yang</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" t="inlineStr"/>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="R145" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr"/>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Wiley</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>physica status solidi (a)</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Then, Han Wui; Zubair, Ahmad; Bader, Samuel; Koirala, Pratik; Beumer, Michael; Vora, Heli; Golani, Prafful; Radosavljevic, Marko</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N146" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" t="inlineStr"/>
+      <c r="Q146" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="R146" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T146" t="inlineStr"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr"/>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Modeling and Validation of Junction Temperature Estimation in High-Power SiC MOSFET Inverters for Electric Vehicle Applications</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Associacao Brasileira de Eletronica de Potencia SOBRAEP</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Eletrônica de Potência</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Willers, Leonardo R.; Da Silva e Silva, Paulo Henrique Alves; Rocha, Lucas R.; Vieira, Rodrigo Padilha</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>10.18618/rep.e202611</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.18618/rep.e202611</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N147" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
+      <c r="P147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr">
+        <is>
+          <t>Modeling and Validation of Junction Temperature Estimation in High-Power SiC MOSFET Inverters for Electric Vehicle Applications</t>
+        </is>
+      </c>
+      <c r="R147" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T147" t="inlineStr"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr"/>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>E-mode digitally recessed p-NiO tri-junction HEMT with
+                    &lt;i&gt;V&lt;/i&gt;
+                    BR of 2.5 kV</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>APL Electronic Devices</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Esteghamat, Amirhossein; Rezaei, Mohammad; Fonollosa, Jon Elipe; Zong, Yuan; Boureau, Victor; Ganeeva, Gulnaz; Matioli, Elison</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>10.1063/5.0314238</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0314238</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N148" t="inlineStr"/>
+      <c r="O148" t="inlineStr"/>
+      <c r="P148" t="inlineStr"/>
+      <c r="Q148" t="inlineStr">
+        <is>
+          <t>E-mode digitally recessed p-NiO tri-junction HEMT with
+                    &lt;i&gt;V&lt;/i&gt;
+                    BR of 2.5 kV</t>
+        </is>
+      </c>
+      <c r="R148" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr"/>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>ENI, FAVOUR</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N149" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
+      <c r="P149" t="inlineStr"/>
+      <c r="Q149" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="R149" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T149" t="inlineStr"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr"/>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Wang, Rutian; Wei, Jiahui; Yu, Yang</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N150" t="inlineStr"/>
+      <c r="O150" t="inlineStr"/>
+      <c r="P150" t="inlineStr"/>
+      <c r="Q150" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="R150" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr"/>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Wiley</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>physica status solidi (a)</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Then, Han Wui; Zubair, Ahmad; Bader, Samuel; Koirala, Pratik; Beumer, Michael; Vora, Heli; Golani, Prafful; Radosavljevic, Marko</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr"/>
+      <c r="P151" t="inlineStr"/>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="R151" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr"/>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>ENI, FAVOUR</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.21203/rs.3.rs-8785842/v1</t>
+        </is>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N152" t="inlineStr"/>
+      <c r="O152" t="inlineStr"/>
+      <c r="P152" t="inlineStr"/>
+      <c r="Q152" t="inlineStr">
+        <is>
+          <t>MATLAB/Simulink Studies on Inverter-Based Systems: Dynamic and Voltage Response Analysis</t>
+        </is>
+      </c>
+      <c r="R152" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T152" t="inlineStr"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr"/>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Wang, Rutian; Wei, Jiahui; Yu, Yang</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19030856</t>
+        </is>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N153" t="inlineStr"/>
+      <c r="O153" t="inlineStr"/>
+      <c r="P153" t="inlineStr"/>
+      <c r="Q153" t="inlineStr">
+        <is>
+          <t>Dual-Output, Hybrid-Clamped, Quasi-Five-Level Inverter and Its Modulation Strategy</t>
+        </is>
+      </c>
+      <c r="R153" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T153" t="inlineStr"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr"/>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Wiley</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>physica status solidi (a)</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Then, Han Wui; Zubair, Ahmad; Bader, Samuel; Koirala, Pratik; Beumer, Michael; Vora, Heli; Golani, Prafful; Radosavljevic, Marko</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/pssa.202500873</t>
+        </is>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N154" t="inlineStr"/>
+      <c r="O154" t="inlineStr"/>
+      <c r="P154" t="inlineStr"/>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>Future of Power and High‐Speed/RF Electronics with Advanced High‐Performance GaN and Heterogeneous Integration with Silicon CMOS</t>
+        </is>
+      </c>
+      <c r="R154" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>2026-02-06</t>
+        </is>
+      </c>
+      <c r="T154" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-07T23:34Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T154"/>
+  <dimension ref="A1:T158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12039,6 +12039,310 @@
       </c>
       <c r="T154" t="inlineStr"/>
     </row>
+    <row r="155">
+      <c r="A155" t="inlineStr"/>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Kroičs, Kaspars; Voitkāns, Jānis</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr"/>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N155" t="inlineStr"/>
+      <c r="O155" t="inlineStr"/>
+      <c r="P155" t="inlineStr"/>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="R155" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="T155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr"/>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Kroičs, Kaspars; Voitkāns, Jānis</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr"/>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N156" t="inlineStr"/>
+      <c r="O156" t="inlineStr"/>
+      <c r="P156" t="inlineStr"/>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="R156" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S156" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="T156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr"/>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Kroičs, Kaspars; Voitkāns, Jānis</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr"/>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N157" t="inlineStr"/>
+      <c r="O157" t="inlineStr"/>
+      <c r="P157" t="inlineStr"/>
+      <c r="Q157" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="R157" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S157" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="T157" t="inlineStr"/>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr"/>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Kroičs, Kaspars; Voitkāns, Jānis</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr"/>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15030717</t>
+        </is>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N158" t="inlineStr"/>
+      <c r="O158" t="inlineStr"/>
+      <c r="P158" t="inlineStr"/>
+      <c r="Q158" t="inlineStr">
+        <is>
+          <t>Overvoltage Suppression Filter Development for GaN Inverter-Fed Electrical Drive with Long Cable Based on Impedance Measurement</t>
+        </is>
+      </c>
+      <c r="R158" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S158" t="inlineStr">
+        <is>
+          <t>2026-02-07</t>
+        </is>
+      </c>
+      <c r="T158" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-10T23:41Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T158"/>
+  <dimension ref="A1:T182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12343,6 +12343,1798 @@
       </c>
       <c r="T158" t="inlineStr"/>
     </row>
+    <row r="159">
+      <c r="A159" t="inlineStr"/>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>openRxiv</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr"/>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Lin, Kai-Chun; Dandin, Marc</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr"/>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N159" t="inlineStr"/>
+      <c r="O159" t="inlineStr"/>
+      <c r="P159" t="inlineStr"/>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="R159" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S159" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr"/>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Transductive Correlation Filter Cell Detection with Pseudo-Label Adaptation for Lab-on-CMOS Time-Lapse Microscopy</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Lin, Ching-Yi; Dandin, Marc</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr"/>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.177074653.37297619/v1</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.177074653.37297619/v1</t>
+        </is>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N160" t="inlineStr"/>
+      <c r="O160" t="inlineStr"/>
+      <c r="P160" t="inlineStr"/>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>Transductive Correlation Filter Cell Detection with Pseudo-Label Adaptation for Lab-on-CMOS Time-Lapse Microscopy</t>
+        </is>
+      </c>
+      <c r="R160" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T160" t="inlineStr"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr"/>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>A multi-conversion mode time-domain temperature sensor in 90-nm CMOS</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Sādhanā</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Chakraborty, Kuntal; Mondal, Abir J</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr"/>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>10.1007/s12046-025-03021-4</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s12046-025-03021-4</t>
+        </is>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N161" t="inlineStr"/>
+      <c r="O161" t="inlineStr"/>
+      <c r="P161" t="inlineStr"/>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>A multi-conversion mode time-domain temperature sensor in 90-nm CMOS</t>
+        </is>
+      </c>
+      <c r="R161" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S161" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T161" t="inlineStr"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr"/>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N162" t="inlineStr"/>
+      <c r="O162" t="inlineStr"/>
+      <c r="P162" t="inlineStr"/>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R162" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T162" t="inlineStr"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr"/>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>An Empirical Evaluation of an Event-Driven Modular Monolithic Architecture Using Apache Kafka for Real-Time AI-Powered Systems</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Amr, Ibrahim; El-Defrawi, Mai</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.177069590.04655255/v1</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.177069590.04655255/v1</t>
+        </is>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N163" t="inlineStr"/>
+      <c r="O163" t="inlineStr"/>
+      <c r="P163" t="inlineStr"/>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>An Empirical Evaluation of an Event-Driven Modular Monolithic Architecture Using Apache Kafka for Real-Time AI-Powered Systems</t>
+        </is>
+      </c>
+      <c r="R163" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr"/>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>openRxiv</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr"/>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Lin, Kai-Chun; Dandin, Marc</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L164" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M164" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N164" t="inlineStr"/>
+      <c r="O164" t="inlineStr"/>
+      <c r="P164" t="inlineStr"/>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="R164" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S164" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr"/>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Transductive Correlation Filter Cell Detection with Pseudo-Label Adaptation for Lab-on-CMOS Time-Lapse Microscopy</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr"/>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Lin, Ching-Yi; Dandin, Marc</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.177074653.37297619/v1</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.177074653.37297619/v1</t>
+        </is>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N165" t="inlineStr"/>
+      <c r="O165" t="inlineStr"/>
+      <c r="P165" t="inlineStr"/>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>Transductive Correlation Filter Cell Detection with Pseudo-Label Adaptation for Lab-on-CMOS Time-Lapse Microscopy</t>
+        </is>
+      </c>
+      <c r="R165" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S165" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr"/>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>A multi-conversion mode time-domain temperature sensor in 90-nm CMOS</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Sādhanā</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Chakraborty, Kuntal; Mondal, Abir J</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>10.1007/s12046-025-03021-4</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s12046-025-03021-4</t>
+        </is>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L166" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M166" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N166" t="inlineStr"/>
+      <c r="O166" t="inlineStr"/>
+      <c r="P166" t="inlineStr"/>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>A multi-conversion mode time-domain temperature sensor in 90-nm CMOS</t>
+        </is>
+      </c>
+      <c r="R166" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S166" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T166" t="inlineStr"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr"/>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L167" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N167" t="inlineStr"/>
+      <c r="O167" t="inlineStr"/>
+      <c r="P167" t="inlineStr"/>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R167" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S167" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr"/>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L168" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N168" t="inlineStr"/>
+      <c r="O168" t="inlineStr"/>
+      <c r="P168" t="inlineStr"/>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R168" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S168" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr"/>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L169" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N169" t="inlineStr"/>
+      <c r="O169" t="inlineStr"/>
+      <c r="P169" t="inlineStr"/>
+      <c r="Q169" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R169" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S169" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr"/>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L170" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M170" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N170" t="inlineStr"/>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" t="inlineStr"/>
+      <c r="Q170" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R170" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S170" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr"/>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr"/>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N171" t="inlineStr"/>
+      <c r="O171" t="inlineStr"/>
+      <c r="P171" t="inlineStr"/>
+      <c r="Q171" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R171" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S171" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr"/>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr"/>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N172" t="inlineStr"/>
+      <c r="O172" t="inlineStr"/>
+      <c r="P172" t="inlineStr"/>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R172" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S172" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T172" t="inlineStr"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr"/>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr"/>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr"/>
+      <c r="O173" t="inlineStr"/>
+      <c r="P173" t="inlineStr"/>
+      <c r="Q173" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R173" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S173" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr"/>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr"/>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr"/>
+      <c r="O174" t="inlineStr"/>
+      <c r="P174" t="inlineStr"/>
+      <c r="Q174" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R174" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S174" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr"/>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>openRxiv</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr"/>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Lin, Kai-Chun; Dandin, Marc</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr"/>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N175" t="inlineStr"/>
+      <c r="O175" t="inlineStr"/>
+      <c r="P175" t="inlineStr"/>
+      <c r="Q175" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="R175" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S175" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T175" t="inlineStr"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr"/>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Transductive Correlation Filter Cell Detection with Pseudo-Label Adaptation for Lab-on-CMOS Time-Lapse Microscopy</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Lin, Ching-Yi; Dandin, Marc</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr"/>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.177074653.37297619/v1</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.177074653.37297619/v1</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N176" t="inlineStr"/>
+      <c r="O176" t="inlineStr"/>
+      <c r="P176" t="inlineStr"/>
+      <c r="Q176" t="inlineStr">
+        <is>
+          <t>Transductive Correlation Filter Cell Detection with Pseudo-Label Adaptation for Lab-on-CMOS Time-Lapse Microscopy</t>
+        </is>
+      </c>
+      <c r="R176" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S176" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T176" t="inlineStr"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>A multi-conversion mode time-domain temperature sensor in 90-nm CMOS</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Springer Science and Business Media LLC</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Sādhanā</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Chakraborty, Kuntal; Mondal, Abir J</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr"/>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>10.1007/s12046-025-03021-4</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1007/s12046-025-03021-4</t>
+        </is>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L177" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M177" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N177" t="inlineStr"/>
+      <c r="O177" t="inlineStr"/>
+      <c r="P177" t="inlineStr"/>
+      <c r="Q177" t="inlineStr">
+        <is>
+          <t>A multi-conversion mode time-domain temperature sensor in 90-nm CMOS</t>
+        </is>
+      </c>
+      <c r="R177" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S177" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T177" t="inlineStr"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr"/>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr"/>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N178" t="inlineStr"/>
+      <c r="O178" t="inlineStr"/>
+      <c r="P178" t="inlineStr"/>
+      <c r="Q178" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R178" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S178" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr"/>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr"/>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N179" t="inlineStr"/>
+      <c r="O179" t="inlineStr"/>
+      <c r="P179" t="inlineStr"/>
+      <c r="Q179" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R179" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S179" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T179" t="inlineStr"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr"/>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N180" t="inlineStr"/>
+      <c r="O180" t="inlineStr"/>
+      <c r="P180" t="inlineStr"/>
+      <c r="Q180" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R180" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S180" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T180" t="inlineStr"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>Applied Physics Letters</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Ueno, Kohei; Fujisawa, Kaito; Fujioka, Hiroshi</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr"/>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0311448</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N181" t="inlineStr"/>
+      <c r="O181" t="inlineStr"/>
+      <c r="P181" t="inlineStr"/>
+      <c r="Q181" t="inlineStr">
+        <is>
+          <t>Ultralow contact resistance of 0.058 Ω mm achieved by pulsed sputtering deposition of regrown degenerately doped GaN contacts for AlGaN/GaN high-electron-mobility transistors</t>
+        </is>
+      </c>
+      <c r="R181" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S181" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr"/>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>openRxiv</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr"/>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Lin, Kai-Chun; Dandin, Marc</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr"/>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.64898/2026.02.05.704137</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N182" t="inlineStr"/>
+      <c r="O182" t="inlineStr"/>
+      <c r="P182" t="inlineStr"/>
+      <c r="Q182" t="inlineStr">
+        <is>
+          <t>Capacitance Sensor Array for Lab-on-CMOS Applications using a Passive RFID Interface</t>
+        </is>
+      </c>
+      <c r="R182" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S182" t="inlineStr">
+        <is>
+          <t>2026-02-10</t>
+        </is>
+      </c>
+      <c r="T182" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-11T23:36Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T182"/>
+  <dimension ref="A1:T184"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14135,6 +14135,158 @@
       </c>
       <c r="T182" t="inlineStr"/>
     </row>
+    <row r="183">
+      <c r="A183" t="inlineStr"/>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>4.11 A/1650 V Sapphire-Substrate GaN MIS-HEMTs with Thin Buffer for Medium-Voltage Power Applications</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Micromachines</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Chen, Changhao; Liu, Yang; Zhou, Xiaowei; Li, Peixian; Zhang, Yongfeng; Yang, Bo; Yang, Zili; Bai, Junchun</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr"/>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>10.3390/mi17020233</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/mi17020233</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N183" t="inlineStr"/>
+      <c r="O183" t="inlineStr"/>
+      <c r="P183" t="inlineStr"/>
+      <c r="Q183" t="inlineStr">
+        <is>
+          <t>4.11 A/1650 V Sapphire-Substrate GaN MIS-HEMTs with Thin Buffer for Medium-Voltage Power Applications</t>
+        </is>
+      </c>
+      <c r="R183" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S183" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="T183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr"/>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>High-Performance Sensorless Control of a Dual-Inverter Doubly Fed Induction Motor for Electric Vehicle Traction Using a Sliding-Mode Observer</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>Automation</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Zerzeri, Mouna; Khedher, Adel</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr"/>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>10.3390/automation7010031</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/automation7010031</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N184" t="inlineStr"/>
+      <c r="O184" t="inlineStr"/>
+      <c r="P184" t="inlineStr"/>
+      <c r="Q184" t="inlineStr">
+        <is>
+          <t>High-Performance Sensorless Control of a Dual-Inverter Doubly Fed Induction Motor for Electric Vehicle Traction Using a Sliding-Mode Observer</t>
+        </is>
+      </c>
+      <c r="R184" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S184" t="inlineStr">
+        <is>
+          <t>2026-02-11</t>
+        </is>
+      </c>
+      <c r="T184" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-12T23:33Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T184"/>
+  <dimension ref="A1:T190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14287,6 +14287,462 @@
       </c>
       <c r="T184" t="inlineStr"/>
     </row>
+    <row r="185">
+      <c r="A185" t="inlineStr"/>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Robust μ-Synthesis Grid-Side Control for Inverter-Based Resources in Weak Grids</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Kim, Woo-Jung; Lee, Yu-Seok; Chun, Yeong-Han</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr"/>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>10.3390/en19040946</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19040946</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N185" t="inlineStr"/>
+      <c r="O185" t="inlineStr"/>
+      <c r="P185" t="inlineStr"/>
+      <c r="Q185" t="inlineStr">
+        <is>
+          <t>Robust μ-Synthesis Grid-Side Control for Inverter-Based Resources in Weak Grids</t>
+        </is>
+      </c>
+      <c r="R185" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S185" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="T185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr"/>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Inductance and capacitance parasitic prediction thanks to data analysis applied to Si and SiC MOSFET wide frequency band characterization</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>Microelectronics Reliability</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Vidal, P.-E.; Viné, G.; Baffreau, S.; Gopishetti, A.; Le, T.L.</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr"/>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>10.1016/j.microrel.2026.116047</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.microrel.2026.116047</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N186" t="inlineStr"/>
+      <c r="O186" t="inlineStr"/>
+      <c r="P186" t="inlineStr"/>
+      <c r="Q186" t="inlineStr">
+        <is>
+          <t>Inductance and capacitance parasitic prediction thanks to data analysis applied to Si and SiC MOSFET wide frequency band characterization</t>
+        </is>
+      </c>
+      <c r="R186" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S186" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="T186" t="inlineStr"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr"/>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Inductance and capacitance parasitic prediction thanks to data analysis applied to Si and SiC MOSFET wide frequency band characterization</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>Microelectronics Reliability</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Vidal, P.-E.; Viné, G.; Baffreau, S.; Gopishetti, A.; Le, T.L.</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr"/>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>10.1016/j.microrel.2026.116047</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.microrel.2026.116047</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M187" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N187" t="inlineStr"/>
+      <c r="O187" t="inlineStr"/>
+      <c r="P187" t="inlineStr"/>
+      <c r="Q187" t="inlineStr">
+        <is>
+          <t>Inductance and capacitance parasitic prediction thanks to data analysis applied to Si and SiC MOSFET wide frequency band characterization</t>
+        </is>
+      </c>
+      <c r="R187" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S187" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="T187" t="inlineStr"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr"/>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Robust μ-Synthesis Grid-Side Control for Inverter-Based Resources in Weak Grids</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Kim, Woo-Jung; Lee, Yu-Seok; Chun, Yeong-Han</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr"/>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>10.3390/en19040946</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19040946</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N188" t="inlineStr"/>
+      <c r="O188" t="inlineStr"/>
+      <c r="P188" t="inlineStr"/>
+      <c r="Q188" t="inlineStr">
+        <is>
+          <t>Robust μ-Synthesis Grid-Side Control for Inverter-Based Resources in Weak Grids</t>
+        </is>
+      </c>
+      <c r="R188" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S188" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="T188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr"/>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Robust μ-Synthesis Grid-Side Control for Inverter-Based Resources in Weak Grids</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Kim, Woo-Jung; Lee, Yu-Seok; Chun, Yeong-Han</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr"/>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>10.3390/en19040946</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19040946</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N189" t="inlineStr"/>
+      <c r="O189" t="inlineStr"/>
+      <c r="P189" t="inlineStr"/>
+      <c r="Q189" t="inlineStr">
+        <is>
+          <t>Robust μ-Synthesis Grid-Side Control for Inverter-Based Resources in Weak Grids</t>
+        </is>
+      </c>
+      <c r="R189" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S189" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="T189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr"/>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Experimental Investigation of Upstream Water-Level Dynamics for a Standard Open-Channel Sluice Gate and a Simplified Model</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Li, Dongyan; Lv, Mouchao; Li, Hao; Jiang, Mingliang; Zhang, Wenzheng; Wang, Yingying; Qin, Jingtao</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr"/>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>10.3390/w18040476</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/w18040476</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M190" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N190" t="inlineStr"/>
+      <c r="O190" t="inlineStr"/>
+      <c r="P190" t="inlineStr"/>
+      <c r="Q190" t="inlineStr">
+        <is>
+          <t>Experimental Investigation of Upstream Water-Level Dynamics for a Standard Open-Channel Sluice Gate and a Simplified Model</t>
+        </is>
+      </c>
+      <c r="R190" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S190" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="T190" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-13T23:35Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T190"/>
+  <dimension ref="A1:T196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14743,6 +14743,462 @@
       </c>
       <c r="T190" t="inlineStr"/>
     </row>
+    <row r="191">
+      <c r="A191" t="inlineStr"/>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Design and Implementation of a Three-Phase Buck-Boost Split-Source Inverter (BSSI)</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Abdulhussein, Yasameen Sh.; Gün, Ayhan</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr"/>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15040808</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15040808</t>
+        </is>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L191" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M191" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N191" t="inlineStr"/>
+      <c r="O191" t="inlineStr"/>
+      <c r="P191" t="inlineStr"/>
+      <c r="Q191" t="inlineStr">
+        <is>
+          <t>Design and Implementation of a Three-Phase Buck-Boost Split-Source Inverter (BSSI)</t>
+        </is>
+      </c>
+      <c r="R191" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S191" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="T191" t="inlineStr"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr"/>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Research on structural reinforcement of AlGaN/GaN HEMT devices under RF stress</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>Nanotechnology</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Liu, Xingjun; Liu, Hongxia; Su, Mengwei; Xing, Dong; Liu, Chang</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr"/>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6528/ae45b0</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6528/ae45b0</t>
+        </is>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L192" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M192" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N192" t="inlineStr"/>
+      <c r="O192" t="inlineStr"/>
+      <c r="P192" t="inlineStr"/>
+      <c r="Q192" t="inlineStr">
+        <is>
+          <t>Research on structural reinforcement of AlGaN/GaN HEMT devices under RF stress</t>
+        </is>
+      </c>
+      <c r="R192" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S192" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="T192" t="inlineStr"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr"/>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Design and Implementation of a Three-Phase Buck-Boost Split-Source Inverter (BSSI)</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Abdulhussein, Yasameen Sh.; Gün, Ayhan</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr"/>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15040808</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15040808</t>
+        </is>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L193" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M193" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N193" t="inlineStr"/>
+      <c r="O193" t="inlineStr"/>
+      <c r="P193" t="inlineStr"/>
+      <c r="Q193" t="inlineStr">
+        <is>
+          <t>Design and Implementation of a Three-Phase Buck-Boost Split-Source Inverter (BSSI)</t>
+        </is>
+      </c>
+      <c r="R193" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S193" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="T193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr"/>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Robust coordinated fault-tolerant control for aerospace multi-motor synchronous drive systems against inverter fault</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>SAGE Publications</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>Measurement and Control</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Han, Xiaodong; Zhang, Dengfeng; Zhao, Li; Lu, Baochun</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr"/>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>10.1177/00202940261419018</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/00202940261419018</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M194" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="N194" t="inlineStr"/>
+      <c r="O194" t="inlineStr"/>
+      <c r="P194" t="inlineStr"/>
+      <c r="Q194" t="inlineStr">
+        <is>
+          <t>Robust coordinated fault-tolerant control for aerospace multi-motor synchronous drive systems against inverter fault</t>
+        </is>
+      </c>
+      <c r="R194" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S194" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="T194" t="inlineStr"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr"/>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Design and Implementation of a Three-Phase Buck-Boost Split-Source Inverter (BSSI)</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Abdulhussein, Yasameen Sh.; Gün, Ayhan</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr"/>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>10.3390/electronics15040808</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/electronics15040808</t>
+        </is>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L195" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M195" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N195" t="inlineStr"/>
+      <c r="O195" t="inlineStr"/>
+      <c r="P195" t="inlineStr"/>
+      <c r="Q195" t="inlineStr">
+        <is>
+          <t>Design and Implementation of a Three-Phase Buck-Boost Split-Source Inverter (BSSI)</t>
+        </is>
+      </c>
+      <c r="R195" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S195" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="T195" t="inlineStr"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr"/>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Skyrmion manipulation and logic gate functionality in transition metal multilayers</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>Journal of Physics D: Applied Physics</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Mukherjee, Tamali; Satya Narayana Murthy, V; Sadhukhan, Banasree</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr"/>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6463/ae45b9</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6463/ae45b9</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N196" t="inlineStr"/>
+      <c r="O196" t="inlineStr"/>
+      <c r="P196" t="inlineStr"/>
+      <c r="Q196" t="inlineStr">
+        <is>
+          <t>Skyrmion manipulation and logic gate functionality in transition metal multilayers</t>
+        </is>
+      </c>
+      <c r="R196" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S196" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="T196" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-16T23:33Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T196"/>
+  <dimension ref="A1:T199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15199,6 +15199,226 @@
       </c>
       <c r="T196" t="inlineStr"/>
     </row>
+    <row r="197">
+      <c r="A197" t="inlineStr"/>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Neuromorphic Multi-LLM Modular Intelligence Architecture: A Systems-Level Path Toward AGI Beyond Monolithic LLM Limits</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr"/>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Mishra, Anindya</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr"/>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.177127405.56163861/v1</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.177127405.56163861/v1</t>
+        </is>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M197" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N197" t="inlineStr"/>
+      <c r="O197" t="inlineStr"/>
+      <c r="P197" t="inlineStr"/>
+      <c r="Q197" t="inlineStr">
+        <is>
+          <t>Neuromorphic Multi-LLM Modular Intelligence Architecture: A Systems-Level Path Toward AGI Beyond Monolithic LLM Limits</t>
+        </is>
+      </c>
+      <c r="R197" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S197" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="T197" t="inlineStr"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr"/>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Neuromorphic Multi-LLM Modular Intelligence Architecture: A Systems-Level Path Toward AGI Beyond Monolithic LLM Limits</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Institute of Electrical and Electronics Engineers (IEEE)</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr"/>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Mishra, Anindya</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr"/>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>10.36227/techrxiv.177127405.56163861/v1</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.36227/techrxiv.177127405.56163861/v1</t>
+        </is>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L198" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M198" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N198" t="inlineStr"/>
+      <c r="O198" t="inlineStr"/>
+      <c r="P198" t="inlineStr"/>
+      <c r="Q198" t="inlineStr">
+        <is>
+          <t>Neuromorphic Multi-LLM Modular Intelligence Architecture: A Systems-Level Path Toward AGI Beyond Monolithic LLM Limits</t>
+        </is>
+      </c>
+      <c r="R198" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S198" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="T198" t="inlineStr"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr"/>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Advances and Perspectives in Gate Dielectric Thin Films for 4H-SiC MOSFETs</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>Materials</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Bai, Zhaopeng; Liang, Jinsong; Ding, Chengxi; Zhou, Zimo; Luo, Man; Gu, Lin; Ma, Hong-Ping; Zhang, Qing-Chun</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr"/>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>10.3390/ma19040766</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/ma19040766</t>
+        </is>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M199" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N199" t="inlineStr"/>
+      <c r="O199" t="inlineStr"/>
+      <c r="P199" t="inlineStr"/>
+      <c r="Q199" t="inlineStr">
+        <is>
+          <t>Advances and Perspectives in Gate Dielectric Thin Films for 4H-SiC MOSFETs</t>
+        </is>
+      </c>
+      <c r="R199" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S199" t="inlineStr">
+        <is>
+          <t>2026-02-16</t>
+        </is>
+      </c>
+      <c r="T199" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-17T23:33Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T199"/>
+  <dimension ref="A1:T216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15419,6 +15419,1298 @@
       </c>
       <c r="T199" t="inlineStr"/>
     </row>
+    <row r="200">
+      <c r="A200" t="inlineStr"/>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 2, The Typology)</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>SAGE Publications</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>Journal of Integrative and Complementary Medicine</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Ijaz, Nadine</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr"/>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>10.1177/27683605251399058</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/27683605251399058</t>
+        </is>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L200" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M200" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N200" t="inlineStr"/>
+      <c r="O200" t="inlineStr"/>
+      <c r="P200" t="inlineStr"/>
+      <c r="Q200" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 2, The Typology)</t>
+        </is>
+      </c>
+      <c r="R200" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S200" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr"/>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 3, Using the Classification Model)</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>SAGE Publications</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>Journal of Integrative and Complementary Medicine</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Ijaz, Nadine</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr"/>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>10.1177/27683605251399056</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/27683605251399056</t>
+        </is>
+      </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L201" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M201" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N201" t="inlineStr"/>
+      <c r="O201" t="inlineStr"/>
+      <c r="P201" t="inlineStr"/>
+      <c r="Q201" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 3, Using the Classification Model)</t>
+        </is>
+      </c>
+      <c r="R201" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S201" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr"/>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>What is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part I, Conceptual Foundations)</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>SAGE Publications</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>Journal of Integrative and Complementary Medicine</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>Ijaz, Nadine</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr"/>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>10.1177/27683605251398692</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/27683605251398692</t>
+        </is>
+      </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L202" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M202" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N202" t="inlineStr"/>
+      <c r="O202" t="inlineStr"/>
+      <c r="P202" t="inlineStr"/>
+      <c r="Q202" t="inlineStr">
+        <is>
+          <t>What is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part I, Conceptual Foundations)</t>
+        </is>
+      </c>
+      <c r="R202" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S202" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr"/>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 2, The Typology)</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>SAGE Publications</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>Journal of Integrative and Complementary Medicine</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Ijaz, Nadine</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr"/>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>10.1177/27683605251399058</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/27683605251399058</t>
+        </is>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L203" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M203" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N203" t="inlineStr"/>
+      <c r="O203" t="inlineStr"/>
+      <c r="P203" t="inlineStr"/>
+      <c r="Q203" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 2, The Typology)</t>
+        </is>
+      </c>
+      <c r="R203" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S203" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr"/>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 3, Using the Classification Model)</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>SAGE Publications</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>Journal of Integrative and Complementary Medicine</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Ijaz, Nadine</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr"/>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>10.1177/27683605251399056</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/27683605251399056</t>
+        </is>
+      </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L204" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M204" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N204" t="inlineStr"/>
+      <c r="O204" t="inlineStr"/>
+      <c r="P204" t="inlineStr"/>
+      <c r="Q204" t="inlineStr">
+        <is>
+          <t>What Is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part 3, Using the Classification Model)</t>
+        </is>
+      </c>
+      <c r="R204" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S204" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr"/>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>What is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part I, Conceptual Foundations)</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>SAGE Publications</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>Journal of Integrative and Complementary Medicine</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Ijaz, Nadine</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr"/>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>10.1177/27683605251398692</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1177/27683605251398692</t>
+        </is>
+      </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L205" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M205" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N205" t="inlineStr"/>
+      <c r="O205" t="inlineStr"/>
+      <c r="P205" t="inlineStr"/>
+      <c r="Q205" t="inlineStr">
+        <is>
+          <t>What is Traditional, Complementary, and Integrative Medicine: An Operational Typology (Part I, Conceptual Foundations)</t>
+        </is>
+      </c>
+      <c r="R205" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S205" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr"/>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Nanotechnology</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Liu, Wenjun; Zhang, Yachao; Wang, Zhizhe; Su, Kai; Zhao, Shenglei; Xu, Shengrui; Zhang, Jinfeng; Yao, Yixin; Wang, Baiqi; Dong, Yaolong; Hao, Yue; Zhang, Jincheng</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr"/>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L206" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M206" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N206" t="inlineStr"/>
+      <c r="O206" t="inlineStr"/>
+      <c r="P206" t="inlineStr"/>
+      <c r="Q206" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="R206" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S206" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr"/>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>Nanotechnology</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Liu, Wenjun; Zhang, Yachao; Wang, Zhizhe; Su, Kai; Zhao, Shenglei; Xu, Shengrui; Zhang, Jinfeng; Yao, Yixin; Wang, Baiqi; Dong, Yaolong; Hao, Yue; Zhang, Jincheng</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr"/>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L207" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M207" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N207" t="inlineStr"/>
+      <c r="O207" t="inlineStr"/>
+      <c r="P207" t="inlineStr"/>
+      <c r="Q207" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="R207" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S207" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr"/>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Nanotechnology</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Liu, Wenjun; Zhang, Yachao; Wang, Zhizhe; Su, Kai; Zhao, Shenglei; Xu, Shengrui; Zhang, Jinfeng; Yao, Yixin; Wang, Baiqi; Dong, Yaolong; Hao, Yue; Zhang, Jincheng</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr"/>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L208" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M208" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N208" t="inlineStr"/>
+      <c r="O208" t="inlineStr"/>
+      <c r="P208" t="inlineStr"/>
+      <c r="Q208" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="R208" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S208" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr"/>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Revealing trap dynamics in p-GaN gate HEMTs: a stretched exponential model for positive and negative bias-temperature instability</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Journal of Physics D: Applied Physics</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Rahman, S. M. Razibur; Rahman, Ehsanur</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr"/>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6463/ae46aa</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6463/ae46aa</t>
+        </is>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L209" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M209" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N209" t="inlineStr"/>
+      <c r="O209" t="inlineStr"/>
+      <c r="P209" t="inlineStr"/>
+      <c r="Q209" t="inlineStr">
+        <is>
+          <t>Revealing trap dynamics in p-GaN gate HEMTs: a stretched exponential model for positive and negative bias-temperature instability</t>
+        </is>
+      </c>
+      <c r="R209" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S209" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr"/>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Investigation of cap layer effects on low-contact-resistance vanadium-based Au-free low-temperature ohmic contacts for AlGaN/GaN HEMT</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Solid-State Electronics</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Xie, Zijing; Ma, Xiao; Li, Xinghuan; Tang, Jun; Wang, Hong</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr"/>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>10.1016/j.sse.2026.109351</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.sse.2026.109351</t>
+        </is>
+      </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L210" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M210" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N210" t="inlineStr"/>
+      <c r="O210" t="inlineStr"/>
+      <c r="P210" t="inlineStr"/>
+      <c r="Q210" t="inlineStr">
+        <is>
+          <t>Investigation of cap layer effects on low-contact-resistance vanadium-based Au-free low-temperature ohmic contacts for AlGaN/GaN HEMT</t>
+        </is>
+      </c>
+      <c r="R210" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S210" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr"/>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Revealing trap dynamics in p-GaN gate HEMTs: a stretched exponential model for positive and negative bias-temperature instability</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Journal of Physics D: Applied Physics</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>Rahman, S. M. Razibur; Rahman, Ehsanur</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr"/>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6463/ae46aa</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6463/ae46aa</t>
+        </is>
+      </c>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L211" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M211" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N211" t="inlineStr"/>
+      <c r="O211" t="inlineStr"/>
+      <c r="P211" t="inlineStr"/>
+      <c r="Q211" t="inlineStr">
+        <is>
+          <t>Revealing trap dynamics in p-GaN gate HEMTs: a stretched exponential model for positive and negative bias-temperature instability</t>
+        </is>
+      </c>
+      <c r="R211" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S211" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr"/>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Investigation of cap layer effects on low-contact-resistance vanadium-based Au-free low-temperature ohmic contacts for AlGaN/GaN HEMT</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Solid-State Electronics</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>Xie, Zijing; Ma, Xiao; Li, Xinghuan; Tang, Jun; Wang, Hong</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr"/>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>10.1016/j.sse.2026.109351</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.sse.2026.109351</t>
+        </is>
+      </c>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L212" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M212" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N212" t="inlineStr"/>
+      <c r="O212" t="inlineStr"/>
+      <c r="P212" t="inlineStr"/>
+      <c r="Q212" t="inlineStr">
+        <is>
+          <t>Investigation of cap layer effects on low-contact-resistance vanadium-based Au-free low-temperature ohmic contacts for AlGaN/GaN HEMT</t>
+        </is>
+      </c>
+      <c r="R212" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S212" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr"/>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Revealing trap dynamics in p-GaN gate HEMTs: a stretched exponential model for positive and negative bias-temperature instability</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>Journal of Physics D: Applied Physics</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Rahman, S. M. Razibur; Rahman, Ehsanur</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr"/>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6463/ae46aa</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6463/ae46aa</t>
+        </is>
+      </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L213" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M213" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N213" t="inlineStr"/>
+      <c r="O213" t="inlineStr"/>
+      <c r="P213" t="inlineStr"/>
+      <c r="Q213" t="inlineStr">
+        <is>
+          <t>Revealing trap dynamics in p-GaN gate HEMTs: a stretched exponential model for positive and negative bias-temperature instability</t>
+        </is>
+      </c>
+      <c r="R213" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S213" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr"/>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>Nanotechnology</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Liu, Wenjun; Zhang, Yachao; Wang, Zhizhe; Su, Kai; Zhao, Shenglei; Xu, Shengrui; Zhang, Jinfeng; Yao, Yixin; Wang, Baiqi; Dong, Yaolong; Hao, Yue; Zhang, Jincheng</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr"/>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L214" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M214" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N214" t="inlineStr"/>
+      <c r="O214" t="inlineStr"/>
+      <c r="P214" t="inlineStr"/>
+      <c r="Q214" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="R214" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S214" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr"/>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Nanotechnology</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Liu, Wenjun; Zhang, Yachao; Wang, Zhizhe; Su, Kai; Zhao, Shenglei; Xu, Shengrui; Zhang, Jinfeng; Yao, Yixin; Wang, Baiqi; Dong, Yaolong; Hao, Yue; Zhang, Jincheng</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr"/>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6528/ae46a5</t>
+        </is>
+      </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L215" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M215" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N215" t="inlineStr"/>
+      <c r="O215" t="inlineStr"/>
+      <c r="P215" t="inlineStr"/>
+      <c r="Q215" t="inlineStr">
+        <is>
+          <t>High-performance GaN HEMTs with over 2 MV/cm breakdown field and 73% PAE via an AlN super back barrier/ultra-thin GaN channel heterostructure</t>
+        </is>
+      </c>
+      <c r="R215" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S215" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr"/>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Investigation of cap layer effects on low-contact-resistance vanadium-based Au-free low-temperature ohmic contacts for AlGaN/GaN HEMT</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Elsevier BV</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Solid-State Electronics</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>Xie, Zijing; Ma, Xiao; Li, Xinghuan; Tang, Jun; Wang, Hong</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr"/>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>10.1016/j.sse.2026.109351</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1016/j.sse.2026.109351</t>
+        </is>
+      </c>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L216" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M216" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N216" t="inlineStr"/>
+      <c r="O216" t="inlineStr"/>
+      <c r="P216" t="inlineStr"/>
+      <c r="Q216" t="inlineStr">
+        <is>
+          <t>Investigation of cap layer effects on low-contact-resistance vanadium-based Au-free low-temperature ohmic contacts for AlGaN/GaN HEMT</t>
+        </is>
+      </c>
+      <c r="R216" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S216" t="inlineStr">
+        <is>
+          <t>2026-02-17</t>
+        </is>
+      </c>
+      <c r="T216" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-18T23:34Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T216"/>
+  <dimension ref="A1:T220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16711,6 +16711,310 @@
       </c>
       <c r="T216" t="inlineStr"/>
     </row>
+    <row r="217">
+      <c r="A217" t="inlineStr"/>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Physics-based full-band GaN high-electron-mobility transistor simulation suggests upper bound of LO phonon lifetime</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Journal of Applied Physics</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Dastider, Ankan Ghosh; Grupen, Matt; Tunga, Ashwin; Rakheja, Shaloo</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr"/>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>10.1063/5.0315424</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0315424</t>
+        </is>
+      </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L217" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M217" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="N217" t="inlineStr"/>
+      <c r="O217" t="inlineStr"/>
+      <c r="P217" t="inlineStr"/>
+      <c r="Q217" t="inlineStr">
+        <is>
+          <t>Physics-based full-band GaN high-electron-mobility transistor simulation suggests upper bound of LO phonon lifetime</t>
+        </is>
+      </c>
+      <c r="R217" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S217" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="T217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr"/>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Novel FOM-enhanced sided-shield gate trench MOSFET with super-junction structure</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Semiconductor Science and Technology</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Yu, Hincheung; Sun, Yabin; Li, Xiaojin; Shi, Yanling; Shen, Yang; Ye, Bingyi; Zhang, Yuhang; Liu, Ziyu</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr"/>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6641/ae4777</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6641/ae4777</t>
+        </is>
+      </c>
+      <c r="J218" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L218" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M218" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N218" t="inlineStr"/>
+      <c r="O218" t="inlineStr"/>
+      <c r="P218" t="inlineStr"/>
+      <c r="Q218" t="inlineStr">
+        <is>
+          <t>Novel FOM-enhanced sided-shield gate trench MOSFET with super-junction structure</t>
+        </is>
+      </c>
+      <c r="R218" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S218" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="T218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr"/>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Novel FOM-enhanced sided-shield gate trench MOSFET with super-junction structure</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>IOP Publishing</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Semiconductor Science and Technology</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Yu, Hincheung; Sun, Yabin; Li, Xiaojin; Shi, Yanling; Shen, Yang; Ye, Bingyi; Zhang, Yuhang; Liu, Ziyu</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr"/>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>10.1088/1361-6641/ae4777</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1088/1361-6641/ae4777</t>
+        </is>
+      </c>
+      <c r="J219" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L219" t="inlineStr">
+        <is>
+          <t>TCAD</t>
+        </is>
+      </c>
+      <c r="M219" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N219" t="inlineStr"/>
+      <c r="O219" t="inlineStr"/>
+      <c r="P219" t="inlineStr"/>
+      <c r="Q219" t="inlineStr">
+        <is>
+          <t>Novel FOM-enhanced sided-shield gate trench MOSFET with super-junction structure</t>
+        </is>
+      </c>
+      <c r="R219" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S219" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="T219" t="inlineStr"/>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr"/>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Physics-based full-band GaN high-electron-mobility transistor simulation suggests upper bound of LO phonon lifetime</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Journal of Applied Physics</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Dastider, Ankan Ghosh; Grupen, Matt; Tunga, Ashwin; Rakheja, Shaloo</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr"/>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>10.1063/5.0315424</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0315424</t>
+        </is>
+      </c>
+      <c r="J220" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K220" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L220" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M220" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="N220" t="inlineStr"/>
+      <c r="O220" t="inlineStr"/>
+      <c r="P220" t="inlineStr"/>
+      <c r="Q220" t="inlineStr">
+        <is>
+          <t>Physics-based full-band GaN high-electron-mobility transistor simulation suggests upper bound of LO phonon lifetime</t>
+        </is>
+      </c>
+      <c r="R220" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S220" t="inlineStr">
+        <is>
+          <t>2026-02-18</t>
+        </is>
+      </c>
+      <c r="T220" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-19T23:33Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T220"/>
+  <dimension ref="A1:T229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17015,6 +17015,682 @@
       </c>
       <c r="T220" t="inlineStr"/>
     </row>
+    <row r="221">
+      <c r="A221" t="inlineStr"/>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Current-Summing Multilevel LCC Inverter for Radiated EMI Harmonic Reduction in Wireless Power Transfer</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Khan, Waqar Hussain; Ahn, Dukju</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr"/>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>10.3390/en19041063</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19041063</t>
+        </is>
+      </c>
+      <c r="J221" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K221" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L221" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M221" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N221" t="inlineStr"/>
+      <c r="O221" t="inlineStr"/>
+      <c r="P221" t="inlineStr"/>
+      <c r="Q221" t="inlineStr">
+        <is>
+          <t>Current-Summing Multilevel LCC Inverter for Radiated EMI Harmonic Reduction in Wireless Power Transfer</t>
+        </is>
+      </c>
+      <c r="R221" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S221" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr"/>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Distilling Protein Language Models with Complementary Regularizers</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>openRxiv</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr"/>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>Wijaya, Edward</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr"/>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>10.64898/2026.02.17.706304</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.64898/2026.02.17.706304</t>
+        </is>
+      </c>
+      <c r="J222" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K222" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L222" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M222" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N222" t="inlineStr"/>
+      <c r="O222" t="inlineStr"/>
+      <c r="P222" t="inlineStr"/>
+      <c r="Q222" t="inlineStr">
+        <is>
+          <t>Distilling Protein Language Models with Complementary Regularizers</t>
+        </is>
+      </c>
+      <c r="R222" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S222" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr"/>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Distilling Protein Language Models with Complementary Regularizers</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>openRxiv</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr"/>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>Wijaya, Edward</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr"/>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>10.64898/2026.02.17.706304</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.64898/2026.02.17.706304</t>
+        </is>
+      </c>
+      <c r="J223" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K223" t="inlineStr">
+        <is>
+          <t>Co-integration</t>
+        </is>
+      </c>
+      <c r="L223" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M223" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N223" t="inlineStr"/>
+      <c r="O223" t="inlineStr"/>
+      <c r="P223" t="inlineStr"/>
+      <c r="Q223" t="inlineStr">
+        <is>
+          <t>Distilling Protein Language Models with Complementary Regularizers</t>
+        </is>
+      </c>
+      <c r="R223" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S223" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr"/>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Journal of Applied Physics</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Asteris, Aias; Nguyen, Thai-Son; Chang, Chuan F. C.; Savant, Chandrashekhar; Lonergan, Pierce; Xing, Huili G.; Jena, Debdeep</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr"/>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="J224" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K224" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L224" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M224" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N224" t="inlineStr"/>
+      <c r="O224" t="inlineStr"/>
+      <c r="P224" t="inlineStr"/>
+      <c r="Q224" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="R224" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S224" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr"/>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Journal of Applied Physics</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>Asteris, Aias; Nguyen, Thai-Son; Chang, Chuan F. C.; Savant, Chandrashekhar; Lonergan, Pierce; Xing, Huili G.; Jena, Debdeep</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr"/>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="J225" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K225" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L225" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M225" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N225" t="inlineStr"/>
+      <c r="O225" t="inlineStr"/>
+      <c r="P225" t="inlineStr"/>
+      <c r="Q225" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="R225" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S225" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr"/>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Current-Summing Multilevel LCC Inverter for Radiated EMI Harmonic Reduction in Wireless Power Transfer</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Khan, Waqar Hussain; Ahn, Dukju</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr"/>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>10.3390/en19041063</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19041063</t>
+        </is>
+      </c>
+      <c r="J226" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L226" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M226" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N226" t="inlineStr"/>
+      <c r="O226" t="inlineStr"/>
+      <c r="P226" t="inlineStr"/>
+      <c r="Q226" t="inlineStr">
+        <is>
+          <t>Current-Summing Multilevel LCC Inverter for Radiated EMI Harmonic Reduction in Wireless Power Transfer</t>
+        </is>
+      </c>
+      <c r="R226" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S226" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr"/>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Current-Summing Multilevel LCC Inverter for Radiated EMI Harmonic Reduction in Wireless Power Transfer</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>MDPI AG</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Energies</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>Khan, Waqar Hussain; Ahn, Dukju</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr"/>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>10.3390/en19041063</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.3390/en19041063</t>
+        </is>
+      </c>
+      <c r="J227" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K227" t="inlineStr">
+        <is>
+          <t>Inverter</t>
+        </is>
+      </c>
+      <c r="L227" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M227" t="inlineStr">
+        <is>
+          <t>Contacts</t>
+        </is>
+      </c>
+      <c r="N227" t="inlineStr"/>
+      <c r="O227" t="inlineStr"/>
+      <c r="P227" t="inlineStr"/>
+      <c r="Q227" t="inlineStr">
+        <is>
+          <t>Current-Summing Multilevel LCC Inverter for Radiated EMI Harmonic Reduction in Wireless Power Transfer</t>
+        </is>
+      </c>
+      <c r="R227" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S227" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr"/>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Journal of Applied Physics</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>Asteris, Aias; Nguyen, Thai-Son; Chang, Chuan F. C.; Savant, Chandrashekhar; Lonergan, Pierce; Xing, Huili G.; Jena, Debdeep</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr"/>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="J228" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K228" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L228" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M228" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N228" t="inlineStr"/>
+      <c r="O228" t="inlineStr"/>
+      <c r="P228" t="inlineStr"/>
+      <c r="Q228" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="R228" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S228" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr"/>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>AIP Publishing</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Journal of Applied Physics</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>Asteris, Aias; Nguyen, Thai-Son; Chang, Chuan F. C.; Savant, Chandrashekhar; Lonergan, Pierce; Xing, Huili G.; Jena, Debdeep</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr"/>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1063/5.0312252</t>
+        </is>
+      </c>
+      <c r="J229" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K229" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L229" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M229" t="inlineStr">
+        <is>
+          <t>Gate Stack</t>
+        </is>
+      </c>
+      <c r="N229" t="inlineStr"/>
+      <c r="O229" t="inlineStr"/>
+      <c r="P229" t="inlineStr"/>
+      <c r="Q229" t="inlineStr">
+        <is>
+          <t>High mobility multiple-channel AlScN/GaN heterostructures</t>
+        </is>
+      </c>
+      <c r="R229" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S229" t="inlineStr">
+        <is>
+          <t>2026-02-19</t>
+        </is>
+      </c>
+      <c r="T229" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
IKD update: GaN CMOS 2026-02-21T23:28Z
</commit_message>
<xml_diff>
--- a/01_literature/IKD_Literature_Master.xlsx
+++ b/01_literature/IKD_Literature_Master.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T229"/>
+  <dimension ref="A1:T230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17691,6 +17691,86 @@
       </c>
       <c r="T229" t="inlineStr"/>
     </row>
+    <row r="230">
+      <c r="A230" t="inlineStr"/>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Investigation of Thermal Characteristics of Multilayer Heterostructures for Enhanced
+                    &lt;scp&gt;GaN HEMT&lt;/scp&gt;
+                    Reliability</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>2026</v>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Wiley</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>International Journal of Numerical Modelling: Electronic Networks, Devices and Fields</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>Mzoughi, Haykel; Nasri, Faouzi; El Amraoui, Lilia</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr"/>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>10.1002/jnm.70154</t>
+        </is>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1002/jnm.70154</t>
+        </is>
+      </c>
+      <c r="J230" t="inlineStr">
+        <is>
+          <t>Journal</t>
+        </is>
+      </c>
+      <c r="K230" t="inlineStr">
+        <is>
+          <t>n-FET</t>
+        </is>
+      </c>
+      <c r="L230" t="inlineStr">
+        <is>
+          <t>Experiment</t>
+        </is>
+      </c>
+      <c r="M230" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="N230" t="inlineStr"/>
+      <c r="O230" t="inlineStr"/>
+      <c r="P230" t="inlineStr"/>
+      <c r="Q230" t="inlineStr">
+        <is>
+          <t>Investigation of Thermal Characteristics of Multilayer Heterostructures for Enhanced
+                    &lt;scp&gt;GaN HEMT&lt;/scp&gt;
+                    Reliability</t>
+        </is>
+      </c>
+      <c r="R230" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="S230" t="inlineStr">
+        <is>
+          <t>2026-02-21</t>
+        </is>
+      </c>
+      <c r="T230" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>